<commit_message>
Adding excel upload for adding Funds
</commit_message>
<xml_diff>
--- a/src/public/addFundTemplate.xlsx
+++ b/src/public/addFundTemplate.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Craig\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Craig\fintechWorkflowTracker\src\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{652291E5-3794-4AA2-B54B-3706E4506AE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{433A0314-BC4C-4AF6-B032-A0D8D4E6F294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3B7DD68C-432E-4BC2-8F3C-800A447499F1}"/>
   </bookViews>
@@ -93,9 +93,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="dd/mm"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -133,7 +130,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,21 +447,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C317488-5C58-46DE-AA33-4E38F8047EF5}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -473,7 +468,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>44926</v>
+        <v>45291</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -489,7 +484,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1">
-        <v>45107</v>
+        <v>45291</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -497,7 +492,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1">
-        <v>45108</v>
+        <v>45292</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -505,7 +500,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1">
-        <v>45109</v>
+        <v>45293</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -513,7 +508,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="1">
-        <v>45110</v>
+        <v>45294</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -521,7 +516,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="1">
-        <v>45111</v>
+        <v>45295</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -529,7 +524,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="1">
-        <v>45112</v>
+        <v>45296</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -537,7 +532,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="1">
-        <v>45113</v>
+        <v>45297</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -545,7 +540,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="1">
-        <v>45114</v>
+        <v>45298</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -553,7 +548,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="1">
-        <v>45115</v>
+        <v>45299</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -561,7 +556,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="1">
-        <v>45116</v>
+        <v>45300</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -569,7 +564,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="1">
-        <v>45117</v>
+        <v>45301</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -577,7 +572,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="1">
-        <v>45118</v>
+        <v>45302</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -585,7 +580,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="1">
-        <v>45119</v>
+        <v>45303</v>
       </c>
     </row>
   </sheetData>

</xml_diff>